<commit_message>
Added simulation mode,tests list
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maintenance\Proj650\P650Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6939863-C99A-497C-8CAE-E7E3EEE9CB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAD7BE0-B001-4094-A9E0-CB62AF0DE8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4548" windowWidth="30936" windowHeight="16896" xr2:uid="{AA3BB085-A6DD-440F-924F-C1A46F9AD039}"/>
+    <workbookView xWindow="636" yWindow="1668" windowWidth="21600" windowHeight="11328" xr2:uid="{AA3BB085-A6DD-440F-924F-C1A46F9AD039}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc219550049" localSheetId="0">Sheet1!$B$8</definedName>
+    <definedName name="_Toc219550049" localSheetId="0">Tests!$B$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>Requirement code</t>
   </si>
@@ -126,6 +127,39 @@
   </si>
   <si>
     <t>STO</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>PC support</t>
+  </si>
+  <si>
+    <t>G Core support</t>
+  </si>
+  <si>
+    <t>Testing  level</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Peer Review</t>
+  </si>
+  <si>
+    <t>Demonstration</t>
+  </si>
+  <si>
+    <t>Quantitative</t>
+  </si>
+  <si>
+    <t>Test reference</t>
+  </si>
+  <si>
+    <t>T1001</t>
+  </si>
+  <si>
+    <t>T1002</t>
   </si>
 </sst>
 </file>
@@ -513,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EAFD0FC-D528-4B47-B6B7-8EE26F388B56}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -525,9 +559,11 @@
     <col min="2" max="2" width="23.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.19921875" customWidth="1"/>
     <col min="4" max="4" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.09765625" customWidth="1"/>
+    <col min="6" max="6" width="18.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +576,14 @@
       <c r="D1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -551,8 +593,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -562,8 +607,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -573,8 +621,11 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1004</v>
       </c>
@@ -584,8 +635,14 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1005</v>
       </c>
@@ -595,8 +652,11 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1006</v>
       </c>
@@ -606,8 +666,14 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1007</v>
       </c>
@@ -617,8 +683,11 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1008</v>
       </c>
@@ -628,8 +697,11 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1009</v>
       </c>
@@ -639,8 +711,11 @@
       <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1010</v>
       </c>
@@ -650,8 +725,11 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1011</v>
       </c>
@@ -661,8 +739,11 @@
       <c r="C13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1012</v>
       </c>
@@ -672,8 +753,11 @@
       <c r="C14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1013</v>
       </c>
@@ -683,8 +767,11 @@
       <c r="C15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1014</v>
       </c>
@@ -694,8 +781,11 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1015</v>
       </c>
@@ -705,8 +795,11 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1016</v>
       </c>
@@ -716,8 +809,11 @@
       <c r="C18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1017</v>
       </c>
@@ -727,8 +823,11 @@
       <c r="C19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1018</v>
       </c>
@@ -738,8 +837,11 @@
       <c r="C20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1019</v>
       </c>
@@ -749,8 +851,11 @@
       <c r="C21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1020</v>
       </c>
@@ -759,10 +864,91 @@
       </c>
       <c r="C22" t="s">
         <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1021</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1022</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75EE694E-CA46-49E1-A68E-CA014112EA5A}">
+          <x14:formula1>
+            <xm:f>Tables!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D46B06-064B-4758-AF16-0C93925F40BE}">
+  <dimension ref="A2:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>